<commit_message>
Poor comparison graphics ready.
</commit_message>
<xml_diff>
--- a/data/poor_datasource_comparison_very_good_match.xlsx
+++ b/data/poor_datasource_comparison_very_good_match.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$U$1:$U$10</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>IDEAM</t>
   </si>
@@ -48,16 +51,344 @@
   </si>
   <si>
     <t>Good Time Series Plot</t>
+  </si>
+  <si>
+    <t>eracomparisonideam_198_416_plotgg.rds
+eracomparisonideam_198_416_plotzoo.rds
+eracomparisonideam_198_416_plotxts.rds</t>
+  </si>
+  <si>
+    <t>no
+yes
+no</t>
+  </si>
+  <si>
+    <t>SHOW IN DOC?</t>
+  </si>
+  <si>
+    <t>yes
+mas o menos
+no</t>
+  </si>
+  <si>
+    <t>eracomparisonideam_195_312_plotgg.rds
+eracomparisonideam_195_312_plotxts.rds
+eracomparisonideam_195_312_plotzoo.rds</t>
+  </si>
+  <si>
+    <t>eracomparisonideam_188_78_plotgg.rds
+eracomparisonideam_188_78_plotzoo.rds
+eracomparisonideam_188_78_plotxts.rds</t>
+  </si>
+  <si>
+    <t>na (IDEAM vs IDEAM)
+na (IDEAM vs IDEAM)
+yes (good time series plot)</t>
+  </si>
+  <si>
+    <t>eracomparisonideam_167_312_plotgg.rds
+eracomparisonideam_167_312_plotzoo.rds
+eracomparisonideam_167_312_plotxts.rds</t>
+  </si>
+  <si>
+    <t>no
+no
+no</t>
+  </si>
+  <si>
+    <t>eracomparisonideam_140_360_plotgg.rds
+eracomparisonideam_140_360_plotzoo.rds
+eracomparisonideam_140_360_plotxts.rds</t>
+  </si>
+  <si>
+    <t>eracomparisonideam_136_416_plotgg.rds
+eracomparisonideam_136_416_plotzoo.rds
+eracomparisonideam_136_416_plotxts.rds</t>
+  </si>
+  <si>
+    <t>eracomparisonideam_129_265_plotgg.rds
+eracomparisonideam_129_265_plotzoo.rds
+eracomparisonideam_129_265_plotxts.rds</t>
+  </si>
+  <si>
+    <t>yes
+no
+no</t>
+  </si>
+  <si>
+    <t>-
+-
+tl</t>
+  </si>
+  <si>
+    <t>yes yes yes
+no
+no (IDEAM vs IDEAM)
+yes yes yes</t>
+  </si>
+  <si>
+    <t>eracomparisonisd_712_312_plotgg.rds
+eracomparisonisd_712_312_plotzoo.rds
+eracomparisonisd_7_312_plotxts.rds
+eracomparisonideam_16712_312_plotgg.rds
+eracomparisonideam_16712_312_plotzoo.rds
+eracomparisonideam_167_312_plotxts.rds
+eracomparisonideam_167_312_plotgg.rds
+eracomparisonideam_167_312_plotzoo.rds</t>
+  </si>
+  <si>
+    <t>no
+no
+no
+no
+no
+no
+no (IDEAM vs ISD)
+no (IDEAM vs ISD)</t>
+  </si>
+  <si>
+    <t>eracomparisonideam_14012_360_plotgg.rds
+eracomparisonideam_14012_360_plotzoo.rds
+eracomparisonideam_140_360_plotxts.rds
+eracomparisonideam_140_360_plotgg.rds
+eracomparisonideam_140_360_plotzoo.rds</t>
+  </si>
+  <si>
+    <t>no (+ o -)
+no
+no
+no (+ o -)
+no</t>
+  </si>
+  <si>
+    <t>eracomparisonisd_912_416_plotgg.rds
+eracomparisonisd_912_416_plotzoo.rds
+eracomparisonisd_9_416_plotxts.rds
+eracomparisonideam_13612_416_plotgg.rds
+eracomparisonideam_13612_416_plotzoo.rds
+eracomparisonideam_136_416_plotxts.rds
+eracomparisonideam_136_416_plotgg.rds
+eracomparisonideam_136_416_plotzoo.rds</t>
+  </si>
+  <si>
+    <t>no
+no
+no
+no (+ o -)
+no
+no
+no (IDEAM vs ISD)
+no (IDEAM vs ISD)</t>
+  </si>
+  <si>
+    <t>no
+si (+ o-)
+no (+ o -)
+no (+ o -)
+no
+no</t>
+  </si>
+  <si>
+    <t>yes
+yes (+ o -)
+no (+ o -)
+no (+ o -)</t>
+  </si>
+  <si>
+    <t>no (IDEAM vs IDEAM)
+yes yes yes (this or the one above, not both)
+no
+no (IDEAM vs IDEAM)
+no (IDEM vs IDEAM)</t>
+  </si>
+  <si>
+    <t>yes (+ o -)
+no
+no
+does not work!
+No</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>eracomparisonideam_18813_78_plotgg.rds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+eracomparisonideam_18813_78_plotzoo.rds
+eracomparisonideam_18823_78_plotzoo.rds
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>eracomparisonideam_188_78_plotxts.rds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">eracomparisonideam_18823_78_plotgg.rds
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>eracomparisonideam_18812_78_plotgg.rds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+eracomparisonideam_18812_78_plotzoo.rds
+eracomparisonideam_188_78_plotgg.rds
+eracomparisonideam_188_78_plotzoo.rds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>eracomparisonideam_12912_265_plotgg.rds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+eracomparisonideam_12912_265_plotzoo.rds
+eracomparisonideam_129_265_plotxts.rds
+eracomparisonideam_129_265_plotgg.rds
+eracomparisonideam_129_265_plotzoo.rds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>eracomparisonideam_19512_312_plotgg.rds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>eracomparisonideam_195_312_plotxts.rds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+eracomparisonideam_19512_312_plotzoo.rds
+eracomparisonideam_195_312_plotzoo.rds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">eracomparisonideam_19812_416_plotgg.rds
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>eracomparisonideam_19812_416_plotzoo.rds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+eracomparisonideam_198_416_plotxts.rds
+eracomparisonideam_198_416_plotgg.rds
+eracomparisonideam_198_416_plotzoo.rds
+eracomparisonideam_195_312_plotgg.rds</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,8 +414,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,18 +703,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" customWidth="1"/>
+    <col min="7" max="7" width="47.109375" customWidth="1"/>
+    <col min="8" max="8" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -386,22 +729,31 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
       </c>
+      <c r="U1">
+        <v>153</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>16015501</v>
       </c>
       <c r="C2">
         <v>78</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
         <v>4</v>
       </c>
+      <c r="U2">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>15079010</v>
       </c>
@@ -411,14 +763,32 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
         <v>0</v>
       </c>
-      <c r="N3" t="s">
+      <c r="S3" t="s">
         <v>1</v>
       </c>
+      <c r="U3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>15075501</v>
       </c>
@@ -428,51 +798,92 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" t="s">
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" t="s">
         <v>5</v>
       </c>
+      <c r="U4">
+        <v>129</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>15015120</v>
       </c>
       <c r="C5">
         <v>265</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" t="s">
         <v>3</v>
       </c>
-      <c r="J5" t="s">
+      <c r="O5" t="s">
         <v>2</v>
       </c>
-      <c r="K5" t="s">
+      <c r="P5" t="s">
         <v>6</v>
       </c>
-      <c r="L5" t="s">
+      <c r="Q5" t="s">
         <v>6</v>
       </c>
-      <c r="N5" t="s">
+      <c r="S5" t="s">
         <v>6</v>
       </c>
+      <c r="U5">
+        <v>136</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>29004520</v>
       </c>
       <c r="C6">
         <v>312</v>
       </c>
-      <c r="J6">
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="O6">
         <v>78</v>
       </c>
-      <c r="K6">
+      <c r="P6">
         <v>153</v>
       </c>
-      <c r="L6">
+      <c r="Q6">
         <v>188</v>
       </c>
+      <c r="U6">
+        <v>140</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>800280</v>
       </c>
@@ -482,48 +893,96 @@
       <c r="C7">
         <v>312</v>
       </c>
-      <c r="J7">
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="O7">
         <v>265</v>
       </c>
-      <c r="K7">
+      <c r="P7">
         <v>129</v>
       </c>
+      <c r="U7">
+        <v>167</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>29045000</v>
       </c>
       <c r="C8">
         <v>360</v>
       </c>
-      <c r="J8">
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="O8">
         <v>312</v>
       </c>
-      <c r="K8">
+      <c r="P8">
         <v>167</v>
       </c>
-      <c r="L8">
+      <c r="Q8">
         <v>195</v>
       </c>
-      <c r="N8">
+      <c r="S8">
         <v>7</v>
       </c>
+      <c r="U8">
+        <v>188</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>28025502</v>
       </c>
       <c r="C9">
         <v>416</v>
       </c>
-      <c r="J9">
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="O9">
         <v>360</v>
       </c>
-      <c r="K9">
+      <c r="P9">
         <v>140</v>
       </c>
+      <c r="U9">
+        <v>195</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>800360</v>
       </c>
@@ -533,20 +992,42 @@
       <c r="C10">
         <v>416</v>
       </c>
-      <c r="J10">
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="O10">
         <v>416</v>
       </c>
-      <c r="K10">
+      <c r="P10">
         <v>136</v>
       </c>
-      <c r="L10">
+      <c r="Q10">
         <v>198</v>
       </c>
-      <c r="N10">
+      <c r="S10">
         <v>9</v>
+      </c>
+      <c r="U10">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="U1:U10">
+    <sortState ref="U2:U10">
+      <sortCondition ref="U1:U10"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ready graphic of integration (h  and nh). About to start results POT-PP
</commit_message>
<xml_diff>
--- a/data/poor_datasource_comparison_very_good_match.xlsx
+++ b/data/poor_datasource_comparison_very_good_match.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$U$1:$U$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$R$1:$R$10</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>IDEAM</t>
   </si>
@@ -41,84 +41,13 @@
     <t>265. Col:20. Row:6. Lon:-74.25. Lat:11.25</t>
   </si>
   <si>
-    <t>909. Col:27. Row:19. Lon:-72.5. Lat:8</t>
-  </si>
-  <si>
     <t>ERA5 grid index of interest: 78,  265, 312, 360, 416</t>
   </si>
   <si>
     <t>COLUMN INDEX</t>
   </si>
   <si>
-    <t>Good Time Series Plot</t>
-  </si>
-  <si>
-    <t>eracomparisonideam_198_416_plotgg.rds
-eracomparisonideam_198_416_plotzoo.rds
-eracomparisonideam_198_416_plotxts.rds</t>
-  </si>
-  <si>
-    <t>no
-yes
-no</t>
-  </si>
-  <si>
     <t>SHOW IN DOC?</t>
-  </si>
-  <si>
-    <t>yes
-mas o menos
-no</t>
-  </si>
-  <si>
-    <t>eracomparisonideam_195_312_plotgg.rds
-eracomparisonideam_195_312_plotxts.rds
-eracomparisonideam_195_312_plotzoo.rds</t>
-  </si>
-  <si>
-    <t>eracomparisonideam_188_78_plotgg.rds
-eracomparisonideam_188_78_plotzoo.rds
-eracomparisonideam_188_78_plotxts.rds</t>
-  </si>
-  <si>
-    <t>na (IDEAM vs IDEAM)
-na (IDEAM vs IDEAM)
-yes (good time series plot)</t>
-  </si>
-  <si>
-    <t>eracomparisonideam_167_312_plotgg.rds
-eracomparisonideam_167_312_plotzoo.rds
-eracomparisonideam_167_312_plotxts.rds</t>
-  </si>
-  <si>
-    <t>no
-no
-no</t>
-  </si>
-  <si>
-    <t>eracomparisonideam_140_360_plotgg.rds
-eracomparisonideam_140_360_plotzoo.rds
-eracomparisonideam_140_360_plotxts.rds</t>
-  </si>
-  <si>
-    <t>eracomparisonideam_136_416_plotgg.rds
-eracomparisonideam_136_416_plotzoo.rds
-eracomparisonideam_136_416_plotxts.rds</t>
-  </si>
-  <si>
-    <t>eracomparisonideam_129_265_plotgg.rds
-eracomparisonideam_129_265_plotzoo.rds
-eracomparisonideam_129_265_plotxts.rds</t>
-  </si>
-  <si>
-    <t>yes
-no
-no</t>
-  </si>
-  <si>
-    <t>-
--
-tl</t>
   </si>
   <si>
     <t>yes yes yes
@@ -372,6 +301,21 @@
 eracomparisonideam_198_416_plotzoo.rds
 eracomparisonideam_195_312_plotgg.rds</t>
     </r>
+  </si>
+  <si>
+    <t>RDS FILE (in red for doc)</t>
+  </si>
+  <si>
+    <t>78. Col:29. Row:2. Lon:-72. Lat:12.25</t>
+  </si>
+  <si>
+    <t>312. Col:18. Row:7. Lon:-74.75. Lat:11</t>
+  </si>
+  <si>
+    <t>360. Col:17. Row:8. Lon:-75. Lat:10.75</t>
+  </si>
+  <si>
+    <t>416. Col:24. Row:9. Lon:-73.25. Lat:10.5</t>
   </si>
 </sst>
 </file>
@@ -703,23 +647,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.6640625" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" customWidth="1"/>
-    <col min="7" max="7" width="47.109375" customWidth="1"/>
-    <col min="8" max="8" width="37.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.109375" customWidth="1"/>
+    <col min="6" max="6" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -729,31 +671,34 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
       <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="U1">
+        <v>6</v>
+      </c>
+      <c r="R1">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>16015501</v>
       </c>
       <c r="C2">
         <v>78</v>
       </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2">
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>15079010</v>
       </c>
@@ -761,34 +706,26 @@
         <v>78</v>
       </c>
       <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
+      <c r="G3" s="3"/>
+      <c r="M3" t="s">
+        <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S3" t="s">
         <v>1</v>
       </c>
-      <c r="U3">
+      <c r="R3">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="72" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>15075501</v>
       </c>
@@ -796,94 +733,85 @@
         <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" t="s">
-        <v>5</v>
-      </c>
-      <c r="U4">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4">
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="72" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>15015120</v>
       </c>
       <c r="C5">
         <v>265</v>
       </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="L5" t="s">
         <v>2</v>
       </c>
+      <c r="M5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" t="s">
+        <v>5</v>
+      </c>
       <c r="P5" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>6</v>
-      </c>
-      <c r="S5" t="s">
-        <v>6</v>
-      </c>
-      <c r="U5">
+        <v>5</v>
+      </c>
+      <c r="R5">
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>29004520</v>
       </c>
       <c r="C6">
         <v>312</v>
       </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="O6">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="L6">
         <v>78</v>
       </c>
-      <c r="P6">
+      <c r="M6">
         <v>153</v>
       </c>
-      <c r="Q6">
+      <c r="N6">
         <v>188</v>
       </c>
-      <c r="U6">
+      <c r="R6">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>800280</v>
       </c>
@@ -893,96 +821,87 @@
       <c r="C7">
         <v>312</v>
       </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="O7">
+        <v>9</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="L7">
         <v>265</v>
       </c>
-      <c r="P7">
+      <c r="M7">
         <v>129</v>
       </c>
-      <c r="U7">
+      <c r="R7">
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="72" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>29045000</v>
       </c>
       <c r="C8">
         <v>360</v>
       </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="O8">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="L8">
         <v>312</v>
       </c>
+      <c r="M8">
+        <v>167</v>
+      </c>
+      <c r="N8">
+        <v>195</v>
+      </c>
       <c r="P8">
-        <v>167</v>
-      </c>
-      <c r="Q8">
-        <v>195</v>
-      </c>
-      <c r="S8">
         <v>7</v>
       </c>
-      <c r="U8">
+      <c r="R8">
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>28025502</v>
       </c>
       <c r="C9">
         <v>416</v>
       </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="O9">
+        <v>14</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="L9">
         <v>360</v>
       </c>
-      <c r="P9">
+      <c r="M9">
         <v>140</v>
       </c>
-      <c r="U9">
+      <c r="R9">
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>800360</v>
       </c>
@@ -992,39 +911,36 @@
       <c r="C10">
         <v>416</v>
       </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="O10">
+        <v>13</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="L10">
         <v>416</v>
       </c>
+      <c r="M10">
+        <v>136</v>
+      </c>
+      <c r="N10">
+        <v>198</v>
+      </c>
       <c r="P10">
-        <v>136</v>
-      </c>
-      <c r="Q10">
-        <v>198</v>
-      </c>
-      <c r="S10">
         <v>9</v>
       </c>
-      <c r="U10">
+      <c r="R10">
         <v>198</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="U1:U10">
-    <sortState ref="U2:U10">
-      <sortCondition ref="U1:U10"/>
+  <autoFilter ref="R1:R10">
+    <sortState ref="R2:R10">
+      <sortCondition ref="R1:R10"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>